<commit_message>
Update SearchStatusItem Implement Effects
</commit_message>
<xml_diff>
--- a/Assets/Scripts/1.Abilities/Resources/Documents/CombineAbilities/CombineAbililties.xlsx
+++ b/Assets/Scripts/1.Abilities/Resources/Documents/CombineAbilities/CombineAbililties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\myWorks\Unity-BolierPlate-Codes\Assets\Scripts\1.Abilities\Resources\Documents\CombineAbilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9399B14-843C-4344-A4F7-E353DE473F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232D4438-27C8-46D7-B84C-91AC06ADCCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="10" xr2:uid="{D49C7B43-6E4D-49C2-B7A8-3A3FDB66E59A}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="28800" windowHeight="15345" firstSheet="6" activeTab="9" xr2:uid="{D49C7B43-6E4D-49C2-B7A8-3A3FDB66E59A}"/>
   </bookViews>
   <sheets>
     <sheet name="AbilityResourceInfo" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="12">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,6 +87,10 @@
   </si>
   <si>
     <t>IsPassive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Motivation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -145,11 +149,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,56 +500,56 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -567,15 +571,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA059A84-6AF1-4A91-9346-3006E82BB928}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -585,69 +592,72 @@
       <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -658,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA2C332-826D-4BD9-A029-FA9CA2CE9A0B}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -681,41 +691,41 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -755,51 +765,51 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -841,74 +851,80 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E8:G8"/>
@@ -916,12 +932,6 @@
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -930,15 +940,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F5BC70-149D-4DE7-ACDA-32783B69FAC3}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -948,51 +958,54 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1029,46 +1042,46 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1105,7 +1118,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1117,75 +1130,75 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1218,84 +1231,90 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
@@ -1305,12 +1324,6 @@
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1344,84 +1357,90 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
@@ -1431,12 +1450,6 @@
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>